<commit_message>
adding topleveldomain to history report
</commit_message>
<xml_diff>
--- a/VisibilityGenerator/history_chart.xlsx
+++ b/VisibilityGenerator/history_chart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>data</t>
   </si>
@@ -31,34 +31,22 @@
     <t>domena</t>
   </si>
   <si>
-    <t>onet.pl</t>
-  </si>
-  <si>
-    <t>wp.pl</t>
-  </si>
-  <si>
-    <t>tvn24.pl</t>
-  </si>
-  <si>
-    <t>fakt.pl</t>
-  </si>
-  <si>
     <t>radiozet.pl</t>
   </si>
   <si>
-    <t>rmf24.pl</t>
-  </si>
-  <si>
-    <t>gazeta.pl</t>
-  </si>
-  <si>
-    <t>wyborcza.pl</t>
-  </si>
-  <si>
-    <t>interia.pl</t>
-  </si>
-  <si>
-    <t>se.pl</t>
+    <t>stylzycia.radiozet.pl</t>
+  </si>
+  <si>
+    <t>zdrowie.radiozet.pl</t>
+  </si>
+  <si>
+    <t>wiadomosci.radiozet.pl</t>
+  </si>
+  <si>
+    <t>sport.radiozet.pl</t>
+  </si>
+  <si>
+    <t>biznes.radiozet.pl</t>
   </si>
 </sst>
 </file>
@@ -420,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,16 +436,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>44108.91666666666</v>
+        <v>44136.95833333334</v>
       </c>
       <c r="C2">
-        <v>167689</v>
+        <v>12862</v>
       </c>
       <c r="D2">
-        <v>653456</v>
+        <v>49996</v>
       </c>
       <c r="E2">
-        <v>3148674</v>
+        <v>267801</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -465,16 +453,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>44115.91666666666</v>
+        <v>44143.95833333334</v>
       </c>
       <c r="C3">
-        <v>165765</v>
+        <v>12939</v>
       </c>
       <c r="D3">
-        <v>652103</v>
+        <v>50199</v>
       </c>
       <c r="E3">
-        <v>3130064</v>
+        <v>266924</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -482,16 +470,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>44122.91666666666</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C4">
-        <v>165318</v>
+        <v>12922</v>
       </c>
       <c r="D4">
-        <v>650468</v>
+        <v>50080</v>
       </c>
       <c r="E4">
-        <v>3147868</v>
+        <v>266317</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -499,50 +487,50 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>44129.95833333334</v>
+        <v>44150.95833333334</v>
       </c>
       <c r="C5">
-        <v>166160</v>
+        <v>12898</v>
       </c>
       <c r="D5">
-        <v>645053</v>
+        <v>49885</v>
       </c>
       <c r="E5">
-        <v>3136593</v>
+        <v>263706</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>44108.91666666666</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C6">
-        <v>150852</v>
+        <v>12785</v>
       </c>
       <c r="D6">
-        <v>653460</v>
+        <v>49814</v>
       </c>
       <c r="E6">
-        <v>2642442</v>
+        <v>260335</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>44115.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C7">
-        <v>149260</v>
+        <v>12911</v>
       </c>
       <c r="D7">
-        <v>653415</v>
+        <v>50166</v>
       </c>
       <c r="E7">
-        <v>2637414</v>
+        <v>258472</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -550,16 +538,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>44122.91666666666</v>
+        <v>44143.95833333334</v>
       </c>
       <c r="C8">
-        <v>148276</v>
+        <v>634</v>
       </c>
       <c r="D8">
-        <v>652624</v>
+        <v>2518</v>
       </c>
       <c r="E8">
-        <v>2637022</v>
+        <v>14762</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -567,67 +555,67 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>44129.95833333334</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C9">
-        <v>149134</v>
+        <v>1037</v>
       </c>
       <c r="D9">
-        <v>650199</v>
+        <v>4003</v>
       </c>
       <c r="E9">
-        <v>2618502</v>
+        <v>21388</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>44108.91666666666</v>
+        <v>44150.95833333334</v>
       </c>
       <c r="C10">
-        <v>33742</v>
+        <v>3082</v>
       </c>
       <c r="D10">
-        <v>143150</v>
+        <v>10663</v>
       </c>
       <c r="E10">
-        <v>809888</v>
+        <v>48109</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>44115.91666666666</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C11">
-        <v>34129</v>
+        <v>5393</v>
       </c>
       <c r="D11">
-        <v>145718</v>
+        <v>18337</v>
       </c>
       <c r="E11">
-        <v>817556</v>
+        <v>81998</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>44122.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C12">
-        <v>34136</v>
+        <v>8201</v>
       </c>
       <c r="D12">
-        <v>145300</v>
+        <v>27330</v>
       </c>
       <c r="E12">
-        <v>811738</v>
+        <v>119521</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -635,67 +623,67 @@
         <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>44129.95833333334</v>
+        <v>44136.95833333334</v>
       </c>
       <c r="C13">
-        <v>33765</v>
+        <v>6999</v>
       </c>
       <c r="D13">
-        <v>142545</v>
+        <v>43090</v>
       </c>
       <c r="E13">
-        <v>802904</v>
+        <v>187652</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>44108.91666666666</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C14">
-        <v>45023</v>
+        <v>6954</v>
       </c>
       <c r="D14">
-        <v>168032</v>
+        <v>42909</v>
       </c>
       <c r="E14">
-        <v>758492</v>
+        <v>185762</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>44115.91666666666</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C15">
-        <v>44819</v>
+        <v>6819</v>
       </c>
       <c r="D15">
-        <v>168638</v>
+        <v>42183</v>
       </c>
       <c r="E15">
-        <v>759454</v>
+        <v>182817</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2">
-        <v>44122.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C16">
-        <v>44720</v>
+        <v>6736</v>
       </c>
       <c r="D16">
-        <v>167536</v>
+        <v>42005</v>
       </c>
       <c r="E16">
-        <v>754855</v>
+        <v>183711</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -703,424 +691,305 @@
         <v>8</v>
       </c>
       <c r="B17" s="2">
-        <v>44129.95833333334</v>
+        <v>44136.95833333334</v>
       </c>
       <c r="C17">
-        <v>42592</v>
+        <v>1243</v>
       </c>
       <c r="D17">
-        <v>163034</v>
+        <v>8393</v>
       </c>
       <c r="E17">
-        <v>737485</v>
+        <v>88115</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2">
-        <v>44108.91666666666</v>
+        <v>44143.95833333334</v>
       </c>
       <c r="C18">
-        <v>25924</v>
+        <v>1281</v>
       </c>
       <c r="D18">
-        <v>125858</v>
+        <v>8302</v>
       </c>
       <c r="E18">
-        <v>744401</v>
+        <v>86296</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2">
-        <v>44115.91666666666</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C19">
-        <v>26340</v>
+        <v>1285</v>
       </c>
       <c r="D19">
-        <v>127498</v>
+        <v>8282</v>
       </c>
       <c r="E19">
-        <v>757543</v>
+        <v>85975</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2">
-        <v>44122.91666666666</v>
+        <v>44150.95833333334</v>
       </c>
       <c r="C20">
-        <v>25269</v>
+        <v>1247</v>
       </c>
       <c r="D20">
-        <v>123907</v>
+        <v>8183</v>
       </c>
       <c r="E20">
-        <v>742631</v>
+        <v>85029</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2">
-        <v>44129.95833333334</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C21">
-        <v>25242</v>
+        <v>1197</v>
       </c>
       <c r="D21">
-        <v>123461</v>
+        <v>7942</v>
       </c>
       <c r="E21">
-        <v>738737</v>
+        <v>84030</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2">
-        <v>44108.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C22">
-        <v>7575</v>
+        <v>1214</v>
       </c>
       <c r="D22">
-        <v>36691</v>
+        <v>7877</v>
       </c>
       <c r="E22">
-        <v>293011</v>
+        <v>83717</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2">
-        <v>44115.91666666666</v>
+        <v>44136.95833333334</v>
       </c>
       <c r="C23">
-        <v>7864</v>
+        <v>1884</v>
       </c>
       <c r="D23">
-        <v>37828</v>
+        <v>10350</v>
       </c>
       <c r="E23">
-        <v>298056</v>
+        <v>63195</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2">
-        <v>44122.91666666666</v>
+        <v>44143.95833333334</v>
       </c>
       <c r="C24">
-        <v>7819</v>
+        <v>1919</v>
       </c>
       <c r="D24">
-        <v>37635</v>
+        <v>10518</v>
       </c>
       <c r="E24">
-        <v>297566</v>
+        <v>63478</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>44129.95833333334</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C25">
-        <v>7660</v>
+        <v>1911</v>
       </c>
       <c r="D25">
-        <v>37048</v>
+        <v>10503</v>
       </c>
       <c r="E25">
-        <v>298457</v>
+        <v>63524</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>44108.91666666666</v>
+        <v>44150.95833333334</v>
       </c>
       <c r="C26">
-        <v>54243</v>
+        <v>1897</v>
       </c>
       <c r="D26">
-        <v>266437</v>
+        <v>10445</v>
       </c>
       <c r="E26">
-        <v>1455992</v>
+        <v>63285</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>44115.91666666666</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C27">
-        <v>54781</v>
+        <v>1880</v>
       </c>
       <c r="D27">
-        <v>268701</v>
+        <v>10341</v>
       </c>
       <c r="E27">
-        <v>1462679</v>
+        <v>63151</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2">
-        <v>44122.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C28">
-        <v>53327</v>
+        <v>1939</v>
       </c>
       <c r="D28">
-        <v>265568</v>
+        <v>10394</v>
       </c>
       <c r="E28">
-        <v>1449983</v>
+        <v>63145</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2">
-        <v>44129.95833333334</v>
+        <v>44136.95833333334</v>
       </c>
       <c r="C29">
-        <v>52165</v>
+        <v>1019</v>
       </c>
       <c r="D29">
-        <v>260839</v>
+        <v>5411</v>
       </c>
       <c r="E29">
-        <v>1439722</v>
+        <v>50723</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2">
-        <v>44108.91666666666</v>
+        <v>44143.95833333334</v>
       </c>
       <c r="C30">
-        <v>65529</v>
+        <v>1016</v>
       </c>
       <c r="D30">
-        <v>381000</v>
+        <v>5387</v>
       </c>
       <c r="E30">
-        <v>2185707</v>
+        <v>50463</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="2">
-        <v>44115.91666666666</v>
+        <v>44144.95833333334</v>
       </c>
       <c r="C31">
-        <v>67926</v>
+        <v>1013</v>
       </c>
       <c r="D31">
-        <v>393051</v>
+        <v>5382</v>
       </c>
       <c r="E31">
-        <v>2212578</v>
+        <v>50383</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2">
-        <v>44122.91666666666</v>
+        <v>44150.95833333334</v>
       </c>
       <c r="C32">
-        <v>68154</v>
+        <v>1005</v>
       </c>
       <c r="D32">
-        <v>395094</v>
+        <v>5365</v>
       </c>
       <c r="E32">
-        <v>2216302</v>
+        <v>50273</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2">
-        <v>44129.95833333334</v>
+        <v>44157.95833333334</v>
       </c>
       <c r="C33">
-        <v>67746</v>
+        <v>980</v>
       </c>
       <c r="D33">
-        <v>390286</v>
+        <v>5383</v>
       </c>
       <c r="E33">
-        <v>2189168</v>
+        <v>50138</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2">
-        <v>44108.91666666666</v>
+        <v>44164.95833333334</v>
       </c>
       <c r="C34">
-        <v>183553</v>
+        <v>1038</v>
       </c>
       <c r="D34">
-        <v>643259</v>
+        <v>5463</v>
       </c>
       <c r="E34">
-        <v>2634673</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="2">
-        <v>44115.91666666666</v>
-      </c>
-      <c r="C35">
-        <v>185781</v>
-      </c>
-      <c r="D35">
-        <v>650816</v>
-      </c>
-      <c r="E35">
-        <v>2648184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="2">
-        <v>44122.91666666666</v>
-      </c>
-      <c r="C36">
-        <v>185305</v>
-      </c>
-      <c r="D36">
-        <v>650384</v>
-      </c>
-      <c r="E36">
-        <v>2682273</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="2">
-        <v>44129.95833333334</v>
-      </c>
-      <c r="C37">
-        <v>182471</v>
-      </c>
-      <c r="D37">
-        <v>644884</v>
-      </c>
-      <c r="E37">
-        <v>2663712</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="2">
-        <v>44108.91666666666</v>
-      </c>
-      <c r="C38">
-        <v>82661</v>
-      </c>
-      <c r="D38">
-        <v>306895</v>
-      </c>
-      <c r="E38">
-        <v>1345835</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="2">
-        <v>44115.91666666666</v>
-      </c>
-      <c r="C39">
-        <v>81674</v>
-      </c>
-      <c r="D39">
-        <v>305600</v>
-      </c>
-      <c r="E39">
-        <v>1332784</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="2">
-        <v>44122.91666666666</v>
-      </c>
-      <c r="C40">
-        <v>80989</v>
-      </c>
-      <c r="D40">
-        <v>304626</v>
-      </c>
-      <c r="E40">
-        <v>1329495</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="2">
-        <v>44129.95833333334</v>
-      </c>
-      <c r="C41">
-        <v>81044</v>
-      </c>
-      <c r="D41">
-        <v>303108</v>
-      </c>
-      <c r="E41">
-        <v>1339674</v>
+        <v>50204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>